<commit_message>
Had to remove egg0089 because it was an egg stuck to egg0088. Replaced with egg0132
</commit_message>
<xml_diff>
--- a/data/incub_geneexp/eggs_to_cull_v3.xlsx
+++ b/data/incub_geneexp/eggs_to_cull_v3.xlsx
@@ -81,15 +81,6 @@
     <t>e017</t>
   </si>
   <si>
-    <t>egg0089</t>
-  </si>
-  <si>
-    <t>c0025</t>
-  </si>
-  <si>
-    <t>dented (see picture), pencil mark</t>
-  </si>
-  <si>
     <t>egg0095</t>
   </si>
   <si>
@@ -268,6 +259,19 @@
   </si>
   <si>
     <t>TC0502 = 1.246g; TC0511 = 1.295g; TC0510 = 1.714g; TC051(4/5) = 0.954g** probably mom</t>
+  </si>
+  <si>
+    <t>egg0123</t>
+  </si>
+  <si>
+    <t>c0037</t>
+  </si>
+  <si>
+    <t>has dent (see picture)
+LD 0195, TC 0451, mass 0.961
+LD 0196, TC 0(34)21, mass 1.367
+LD 0197, TC 1312, mass 0.974
+LD 0198, TC 0(45)53, mass 1.279</t>
   </si>
 </sst>
 </file>
@@ -276,7 +280,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -372,7 +376,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -437,8 +441,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -454,18 +466,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -485,9 +485,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="72">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -519,6 +531,10 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="27" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -551,59 +567,13 @@
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1016,8 +986,8 @@
   </sheetPr>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -1052,16 +1022,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>7</v>
@@ -1076,66 +1046,64 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="16" customHeight="1">
+      <c r="A2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="9">
-        <v>42697</v>
-      </c>
-      <c r="E2" s="8">
-        <v>18</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="C2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="22">
+        <v>42698</v>
+      </c>
+      <c r="E2" s="21">
+        <v>17</v>
+      </c>
+      <c r="F2" s="21">
         <v>23</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
       </c>
       <c r="H2" s="8">
-        <v>19</v>
-      </c>
-      <c r="I2" s="10">
-        <v>42716</v>
+        <v>22</v>
+      </c>
+      <c r="I2" s="9">
+        <v>42720</v>
       </c>
       <c r="J2" s="11">
         <f>H2/4.5+30</f>
-        <v>34.222222222222221</v>
-      </c>
-      <c r="K2" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="L2" s="8">
-        <v>4.46</v>
-      </c>
-      <c r="M2" s="8">
-        <v>8.81</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>22</v>
-      </c>
+        <v>34.888888888888886</v>
+      </c>
+      <c r="K2" s="21">
+        <v>0.111</v>
+      </c>
+      <c r="L2" s="21">
+        <v>5.12</v>
+      </c>
+      <c r="M2" s="21">
+        <v>8.06</v>
+      </c>
+      <c r="N2" s="21"/>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="9">
+        <v>42692</v>
+      </c>
+      <c r="E3" s="8">
         <v>23</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="9">
-        <v>42698</v>
-      </c>
-      <c r="E3" s="8">
-        <v>17</v>
       </c>
       <c r="F3" s="8">
         <v>23</v>
@@ -1144,68 +1112,71 @@
         <v>1</v>
       </c>
       <c r="H3" s="8">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I3" s="9">
-        <v>42720</v>
+        <v>42721</v>
       </c>
       <c r="J3" s="11">
         <f>H3/4.5+30</f>
-        <v>34.888888888888886</v>
+        <v>36.444444444444443</v>
       </c>
       <c r="K3" s="8">
-        <v>0.111</v>
+        <v>0.123</v>
       </c>
       <c r="L3" s="8">
-        <v>5.12</v>
+        <v>5.85</v>
       </c>
       <c r="M3" s="8">
-        <v>8.06</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
-      <c r="A4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="9">
-        <v>42692</v>
-      </c>
-      <c r="E4" s="8">
-        <v>23</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="A4" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="25">
+        <v>42703</v>
+      </c>
+      <c r="E4" s="24">
+        <v>12</v>
+      </c>
+      <c r="F4" s="24">
         <v>23</v>
       </c>
       <c r="G4" s="8">
         <v>1</v>
       </c>
       <c r="H4" s="8">
-        <v>29</v>
-      </c>
-      <c r="I4" s="9">
-        <v>42721</v>
+        <v>19</v>
+      </c>
+      <c r="I4" s="10">
+        <f>D4+H4</f>
+        <v>42722</v>
       </c>
       <c r="J4" s="11">
         <f>H4/4.5+30</f>
-        <v>36.444444444444443</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0.123</v>
-      </c>
-      <c r="L4" s="8">
-        <v>5.85</v>
-      </c>
-      <c r="M4" s="8">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="N4" s="8"/>
+        <v>34.222222222222221</v>
+      </c>
+      <c r="K4" s="24">
+        <v>0.129</v>
+      </c>
+      <c r="L4" s="24">
+        <v>5.08</v>
+      </c>
+      <c r="M4" s="24">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="16" customHeight="1">
       <c r="A5" s="8" t="s">
@@ -1296,13 +1267,13 @@
     </row>
     <row r="7" spans="1:14" ht="16" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9">
         <v>42698</v>
@@ -1339,13 +1310,13 @@
     </row>
     <row r="8" spans="1:14" ht="16" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9">
         <v>42704</v>
@@ -1379,26 +1350,26 @@
         <v>9.6300000000000008</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16" customHeight="1">
-      <c r="A9" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="14">
+      <c r="A9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="23">
         <v>42698</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="17">
         <v>17</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="17">
         <v>23</v>
       </c>
       <c r="G9" s="8">
@@ -1414,26 +1385,26 @@
         <f>H9/4.5+30</f>
         <v>38</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="17">
         <v>0.16400000000000001</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="17">
         <v>8.17</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="17">
         <v>8.61</v>
       </c>
       <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14" ht="16" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="9">
         <v>42705</v>
@@ -1467,26 +1438,26 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16" customHeight="1">
-      <c r="A11" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="A11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="23">
         <v>42698</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="17">
         <v>17</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="17">
         <v>23</v>
       </c>
       <c r="G11" s="8">
@@ -1502,88 +1473,88 @@
         <f>H11/4.5+30</f>
         <v>36</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="17">
         <v>0.186</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="17">
         <v>6.54</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="17">
         <v>8.26</v>
       </c>
-      <c r="N11" s="13" t="s">
-        <v>68</v>
+      <c r="N11" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:14" customFormat="1" ht="16" customHeight="1">
-      <c r="A12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="14">
+      <c r="A12" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="23">
         <v>42701</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="17">
         <v>14</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="17">
         <v>29</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="24">
         <v>1</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="24">
         <v>15</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="25">
         <f>D12+H12</f>
         <v>42716</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="26">
         <f>H12/2.6+30</f>
         <v>35.769230769230766</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="17">
         <v>0.127</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="17">
         <v>5.27</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="17">
         <v>8.19</v>
       </c>
-      <c r="N12" s="13" t="s">
-        <v>74</v>
+      <c r="N12" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:14" customFormat="1" ht="16" customHeight="1">
-      <c r="A13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="23">
         <v>42694</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="17">
         <v>21</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="19">
         <v>29</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="15">
         <v>2</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="15">
         <v>22</v>
       </c>
       <c r="I13" s="9">
@@ -1594,70 +1565,70 @@
         <f>H13/2.6+30</f>
         <v>38.46153846153846</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="17">
         <v>0.108</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="17">
         <v>5.47</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="17">
         <v>7.39</v>
       </c>
-      <c r="N13" s="16"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:14" ht="16" customHeight="1">
-      <c r="A14" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="A14" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="25">
         <v>42698</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="24">
         <v>17</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="24">
         <v>29</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="24">
         <v>1</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="24">
         <v>19</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="25">
         <f>D14+H14</f>
         <v>42717</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="26">
         <f>H14/2.6+30</f>
         <v>37.307692307692307</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="24">
         <v>0.115</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="24">
         <v>5.23</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="24">
         <v>7.67</v>
       </c>
-      <c r="N14" s="16"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" spans="1:14" ht="16" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="9">
         <v>42702</v>
@@ -1691,35 +1662,35 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="N15" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="16" customHeight="1">
+      <c r="A16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="16" customHeight="1">
-      <c r="A16" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="20">
+      <c r="D16" s="14">
         <v>42709</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="15">
         <v>6</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="15">
         <v>29</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="15">
         <v>1</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="15">
         <v>12</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="16">
         <f>D16+12</f>
         <v>42721</v>
       </c>
@@ -1727,28 +1698,28 @@
         <f>H16/2.6+30</f>
         <v>34.615384615384613</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="17">
         <v>0.13500000000000001</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="17">
         <v>5.69</v>
       </c>
-      <c r="M16" s="23">
+      <c r="M16" s="17">
         <v>8.4600000000000009</v>
       </c>
-      <c r="N16" s="24" t="s">
-        <v>61</v>
+      <c r="N16" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="16" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D17" s="9">
         <v>42706</v>
@@ -1782,35 +1753,35 @@
         <v>7.98</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="16" customHeight="1">
-      <c r="A18" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="20">
+      <c r="A18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="14">
         <v>42710</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="15">
         <v>5</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="19">
         <v>29</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="15">
         <v>1</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="15">
         <v>14</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="16">
         <f>D18+14</f>
         <v>42724</v>
       </c>
@@ -1818,28 +1789,28 @@
         <f>H18/2.6+30</f>
         <v>35.384615384615387</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="17">
         <v>0.13700000000000001</v>
       </c>
-      <c r="L18" s="23">
+      <c r="L18" s="17">
         <v>5.83</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="17">
         <v>8.3699999999999992</v>
       </c>
-      <c r="N18" s="24" t="s">
-        <v>57</v>
+      <c r="N18" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D19" s="9">
         <v>42708</v>
@@ -1873,35 +1844,35 @@
         <v>7.33</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="16" customHeight="1">
-      <c r="A20" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="20">
+      <c r="A20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="14">
         <v>42714</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="15">
         <v>1</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="19">
         <v>29</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="15">
         <v>1</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="15">
         <v>12</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="16">
         <f>D20+12</f>
         <v>42726</v>
       </c>
@@ -1909,28 +1880,28 @@
         <f>H20/2.6+30</f>
         <v>34.615384615384613</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="17">
         <v>0.13400000000000001</v>
       </c>
-      <c r="L20" s="23">
+      <c r="L20" s="17">
         <v>5.36</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="17">
         <v>8.35</v>
       </c>
-      <c r="N20" s="24" t="s">
-        <v>41</v>
+      <c r="N20" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="16" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21" s="9">
         <v>42711</v>
@@ -1964,34 +1935,39 @@
         <v>8.76</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="16" customHeight="1">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2">
-        <f t="shared" ref="H22" si="0">AVERAGE(H2:H21)</f>
-        <v>22.6</v>
+        <f>AVERAGE(H3:H21)</f>
+        <v>22.631578947368421</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2">
-        <f>AVERAGE(J2:J21)</f>
-        <v>36.353846153846156</v>
-      </c>
-      <c r="K22" s="26">
-        <f t="shared" ref="K22:M22" si="1">AVERAGE(K2:K21)</f>
-        <v>0.14099999999999999</v>
+        <f>AVERAGE(J3:J21)</f>
+        <v>36.430949167791276</v>
+      </c>
+      <c r="K22" s="20">
+        <f>AVERAGE(K3:K21)</f>
+        <v>0.13673684210526316</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="1"/>
-        <v>5.628000000000001</v>
+        <f>AVERAGE(L3:L21)</f>
+        <v>5.6873684210526321</v>
       </c>
       <c r="M22" s="1">
-        <f t="shared" si="1"/>
-        <v>8.3330000000000002</v>
-      </c>
+        <f>AVERAGE(M3:M21)</f>
+        <v>8.3589473684210525</v>
+      </c>
+      <c r="N22" s="27"/>
     </row>
   </sheetData>
   <sortState ref="A2:N22">
@@ -1999,26 +1975,29 @@
     <sortCondition ref="I2:I22"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B22:B1048576 B1:B2 B4:B8 B12 B10 B14:B20">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+  <conditionalFormatting sqref="B22:B1048576 B1 B4:B8 B12 B10 B14:B20">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="45" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Swapped out egg0044 with egg0015 because egg0043 is from the same clutch as egg0044
</commit_message>
<xml_diff>
--- a/data/incub_geneexp/eggs_to_cull_v3.xlsx
+++ b/data/incub_geneexp/eggs_to_cull_v3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>egg_id</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>egg_notes</t>
-  </si>
-  <si>
-    <t>egg0044</t>
-  </si>
-  <si>
-    <t>c0012</t>
   </si>
   <si>
     <t>e059</t>
@@ -272,6 +266,18 @@
 LD 0196, TC 0(34)21, mass 1.367
 LD 0197, TC 1312, mass 0.974
 LD 0198, TC 0(45)53, mass 1.279</t>
+  </si>
+  <si>
+    <t>egg0115</t>
+  </si>
+  <si>
+    <t>c0034</t>
+  </si>
+  <si>
+    <t>TC0552: 1.105
+TC0452: 1.111
+TC0451:1.560
+TC(235)111: 1.363</t>
   </si>
 </sst>
 </file>
@@ -352,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -375,8 +381,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -449,8 +466,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -498,8 +521,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="78">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -535,6 +566,9 @@
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="27" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -571,9 +605,22 @@
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -984,10 +1031,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="M1" sqref="A1:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
@@ -1022,16 +1069,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>7</v>
@@ -1048,13 +1095,13 @@
     </row>
     <row r="2" spans="1:14" s="5" customFormat="1" ht="16" customHeight="1">
       <c r="A2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="22">
         <v>42698</v>
@@ -1075,7 +1122,7 @@
         <v>42720</v>
       </c>
       <c r="J2" s="11">
-        <f>H2/4.5+30</f>
+        <f t="shared" ref="J2:J11" si="0">H2/4.5+30</f>
         <v>34.888888888888886</v>
       </c>
       <c r="K2" s="21">
@@ -1091,13 +1138,13 @@
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="9">
         <v>42692</v>
@@ -1118,7 +1165,7 @@
         <v>42721</v>
       </c>
       <c r="J3" s="11">
-        <f>H3/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>36.444444444444443</v>
       </c>
       <c r="K3" s="8">
@@ -1134,13 +1181,13 @@
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="25">
         <v>42703</v>
@@ -1162,7 +1209,7 @@
         <v>42722</v>
       </c>
       <c r="J4" s="11">
-        <f>H4/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>34.222222222222221</v>
       </c>
       <c r="K4" s="24">
@@ -1175,26 +1222,26 @@
         <v>9.0299999999999994</v>
       </c>
       <c r="N4" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="16" customHeight="1">
-      <c r="A5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9">
-        <v>42690</v>
-      </c>
-      <c r="E5" s="8">
-        <v>25</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="29">
+        <v>42701</v>
+      </c>
+      <c r="E5" s="24">
+        <v>14</v>
+      </c>
+      <c r="F5" s="24">
         <v>23</v>
       </c>
       <c r="G5" s="8">
@@ -1203,34 +1250,36 @@
       <c r="H5" s="8">
         <v>32</v>
       </c>
-      <c r="I5" s="9">
-        <f>D5+H5</f>
-        <v>42722</v>
+      <c r="I5" s="10">
+        <f>D5+32</f>
+        <v>42733</v>
       </c>
       <c r="J5" s="11">
-        <f>H5/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>37.111111111111114</v>
       </c>
-      <c r="K5" s="8">
-        <v>0.128</v>
-      </c>
-      <c r="L5" s="8">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="M5" s="8">
-        <v>9.16</v>
-      </c>
-      <c r="N5" s="8"/>
+      <c r="K5">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="L5">
+        <v>5.66</v>
+      </c>
+      <c r="M5">
+        <v>8.14</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="16" customHeight="1">
       <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="9">
         <v>42696</v>
@@ -1251,7 +1300,7 @@
         <v>42727</v>
       </c>
       <c r="J6" s="11">
-        <f>H6/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>36.888888888888886</v>
       </c>
       <c r="K6" s="8">
@@ -1267,13 +1316,13 @@
     </row>
     <row r="7" spans="1:14" ht="16" customHeight="1">
       <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="D7" s="9">
         <v>42698</v>
@@ -1294,7 +1343,7 @@
         <v>42729</v>
       </c>
       <c r="J7" s="11">
-        <f>H7/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>36.888888888888886</v>
       </c>
       <c r="K7" s="8">
@@ -1310,13 +1359,13 @@
     </row>
     <row r="8" spans="1:14" ht="16" customHeight="1">
       <c r="A8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="D8" s="9">
         <v>42704</v>
@@ -1337,7 +1386,7 @@
         <v>42731</v>
       </c>
       <c r="J8" s="11">
-        <f>H8/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="K8" s="8">
@@ -1350,18 +1399,18 @@
         <v>9.6300000000000008</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="16" customHeight="1">
       <c r="A9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>68</v>
       </c>
       <c r="D9" s="23">
         <v>42698</v>
@@ -1382,7 +1431,7 @@
         <v>42732</v>
       </c>
       <c r="J9" s="11">
-        <f>H9/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="K9" s="17">
@@ -1398,13 +1447,13 @@
     </row>
     <row r="10" spans="1:14" ht="16" customHeight="1">
       <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="D10" s="9">
         <v>42705</v>
@@ -1425,7 +1474,7 @@
         <v>42739</v>
       </c>
       <c r="J10" s="11">
-        <f>H10/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>37.555555555555557</v>
       </c>
       <c r="K10" s="8">
@@ -1438,18 +1487,18 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="23">
         <v>42698</v>
@@ -1470,7 +1519,7 @@
         <v>42740</v>
       </c>
       <c r="J11" s="11">
-        <f>H11/4.5+30</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="K11" s="17">
@@ -1483,18 +1532,18 @@
         <v>8.26</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:14" customFormat="1" ht="16" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="23">
         <v>42701</v>
@@ -1516,7 +1565,7 @@
         <v>42716</v>
       </c>
       <c r="J12" s="26">
-        <f>H12/2.6+30</f>
+        <f t="shared" ref="J12:J21" si="1">H12/2.6+30</f>
         <v>35.769230769230766</v>
       </c>
       <c r="K12" s="17">
@@ -1529,18 +1578,18 @@
         <v>8.19</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:14" customFormat="1" ht="16" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="23">
         <v>42694</v>
@@ -1562,7 +1611,7 @@
         <v>42716</v>
       </c>
       <c r="J13" s="11">
-        <f>H13/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>38.46153846153846</v>
       </c>
       <c r="K13" s="17">
@@ -1578,13 +1627,13 @@
     </row>
     <row r="14" spans="1:14" ht="16" customHeight="1">
       <c r="A14" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" s="25">
         <v>42698</v>
@@ -1606,7 +1655,7 @@
         <v>42717</v>
       </c>
       <c r="J14" s="26">
-        <f>H14/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>37.307692307692307</v>
       </c>
       <c r="K14" s="24">
@@ -1622,13 +1671,13 @@
     </row>
     <row r="15" spans="1:14" ht="16" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="9">
         <v>42702</v>
@@ -1649,7 +1698,7 @@
         <v>42720</v>
       </c>
       <c r="J15" s="11">
-        <f>H15/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>36.92307692307692</v>
       </c>
       <c r="K15" s="8">
@@ -1662,18 +1711,18 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="16" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="14">
         <v>42709</v>
@@ -1695,7 +1744,7 @@
         <v>42721</v>
       </c>
       <c r="J16" s="11">
-        <f>H16/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>34.615384615384613</v>
       </c>
       <c r="K16" s="17">
@@ -1708,18 +1757,18 @@
         <v>8.4600000000000009</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="16" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="9">
         <v>42706</v>
@@ -1740,7 +1789,7 @@
         <v>42723</v>
       </c>
       <c r="J17" s="11">
-        <f>H17/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>36.53846153846154</v>
       </c>
       <c r="K17" s="8">
@@ -1753,18 +1802,18 @@
         <v>7.98</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="16" customHeight="1">
       <c r="A18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="14">
         <v>42710</v>
@@ -1786,7 +1835,7 @@
         <v>42724</v>
       </c>
       <c r="J18" s="11">
-        <f>H18/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>35.384615384615387</v>
       </c>
       <c r="K18" s="17">
@@ -1799,18 +1848,18 @@
         <v>8.3699999999999992</v>
       </c>
       <c r="N18" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="9">
         <v>42708</v>
@@ -1831,7 +1880,7 @@
         <v>42725</v>
       </c>
       <c r="J19" s="11">
-        <f>H19/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>36.53846153846154</v>
       </c>
       <c r="K19" s="8">
@@ -1844,18 +1893,18 @@
         <v>7.33</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="16" customHeight="1">
       <c r="A20" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="14">
         <v>42714</v>
@@ -1877,7 +1926,7 @@
         <v>42726</v>
       </c>
       <c r="J20" s="11">
-        <f>H20/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>34.615384615384613</v>
       </c>
       <c r="K20" s="17">
@@ -1890,18 +1939,18 @@
         <v>8.35</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="16" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" s="9">
         <v>42711</v>
@@ -1922,7 +1971,7 @@
         <v>42729</v>
       </c>
       <c r="J21" s="11">
-        <f>H21/2.6+30</f>
+        <f t="shared" si="1"/>
         <v>36.92307692307692</v>
       </c>
       <c r="K21" s="8">
@@ -1935,11 +1984,11 @@
         <v>8.76</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="16" customHeight="1">
-      <c r="A22" s="27"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
@@ -1957,17 +2006,20 @@
       </c>
       <c r="K22" s="20">
         <f>AVERAGE(K3:K21)</f>
-        <v>0.13673684210526316</v>
+        <v>0.13705263157894734</v>
       </c>
       <c r="L22" s="1">
         <f>AVERAGE(L3:L21)</f>
-        <v>5.6873684210526321</v>
+        <v>5.7168421052631571</v>
       </c>
       <c r="M22" s="1">
         <f>AVERAGE(M3:M21)</f>
-        <v>8.3589473684210525</v>
+        <v>8.3052631578947373</v>
       </c>
       <c r="N22" s="27"/>
+    </row>
+    <row r="23" spans="1:14" ht="16" customHeight="1">
+      <c r="A23" s="32"/>
     </row>
   </sheetData>
   <sortState ref="A2:N22">
@@ -1975,25 +2027,28 @@
     <sortCondition ref="I2:I22"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B22:B1048576 B1 B4:B8 B12 B10 B14:B20">
+  <conditionalFormatting sqref="B22:B1048576 B1 B4 B12 B10 B14:B20 B6:B8">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
+  <conditionalFormatting sqref="B21">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
+  <conditionalFormatting sqref="B11">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
+  <conditionalFormatting sqref="B9">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
+  <conditionalFormatting sqref="B13">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B2">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="B5">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Swapped egg132 for egg130
</commit_message>
<xml_diff>
--- a/data/incub_geneexp/eggs_to_cull_v3.xlsx
+++ b/data/incub_geneexp/eggs_to_cull_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="0" windowWidth="27140" windowHeight="18680" tabRatio="500"/>
+    <workbookView xWindow="4980" yWindow="0" windowWidth="27140" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="eggs_to_cull.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>egg_id</t>
   </si>
@@ -115,9 +115,6 @@
 LD 0208, TC 0510, mass 1.682
 LD 0209, TC 0511, mass 0.963
 LD 0210, TC 0504, mass 1.222</t>
-  </si>
-  <si>
-    <t>egg0132</t>
   </si>
   <si>
     <t>c0040</t>
@@ -187,20 +184,6 @@
     <t>egg0093</t>
   </si>
   <si>
-    <t>egg0145</t>
-  </si>
-  <si>
-    <t>c0044</t>
-  </si>
-  <si>
-    <t>e027</t>
-  </si>
-  <si>
-    <t>LD 0057, TC 0121, mass 1.389
-LD 0126, TC 0303, mass 1.515
-LD 0104, TC 0225</t>
-  </si>
-  <si>
     <t>egg0151</t>
   </si>
   <si>
@@ -279,16 +262,27 @@
 TC0451:1.560
 TC(235)111: 1.363</t>
   </si>
+  <si>
+    <t>egg0130</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>egg0110</t>
+  </si>
+  <si>
+    <t>c0031</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -344,6 +338,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -388,12 +389,14 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,11 +475,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="27"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,7 +522,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -517,20 +530,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="90">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -569,6 +601,12 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="27" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -608,19 +646,15 @@
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1033,1007 +1067,985 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="M1" sqref="A1:M21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="5" width="10.83203125" style="3" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" style="3"/>
-    <col min="9" max="9" width="14.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="5" width="10.83203125" style="2" customWidth="1"/>
+    <col min="6" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="1"/>
-    <col min="11" max="13" width="10.83203125" style="3"/>
-    <col min="14" max="14" width="132.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="3"/>
+    <col min="11" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="132.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="16" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="16" customHeight="1">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
+      <c r="A2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="20">
         <v>42698</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="19">
         <v>17</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="19">
         <v>23</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>22</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>42720</v>
       </c>
-      <c r="J2" s="11">
-        <f t="shared" ref="J2:J11" si="0">H2/4.5+30</f>
+      <c r="J2" s="10">
+        <f>H2/4.5+30</f>
         <v>34.888888888888886</v>
       </c>
-      <c r="K2" s="21">
+      <c r="K2" s="19">
         <v>0.111</v>
       </c>
-      <c r="L2" s="21">
+      <c r="L2" s="19">
         <v>5.12</v>
       </c>
-      <c r="M2" s="21">
+      <c r="M2" s="19">
         <v>8.06</v>
       </c>
-      <c r="N2" s="21"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14" ht="16" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>42692</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>23</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>23</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>29</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>42721</v>
       </c>
-      <c r="J3" s="11">
-        <f t="shared" si="0"/>
+      <c r="J3" s="10">
+        <f>H3/4.5+30</f>
         <v>36.444444444444443</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <v>0.123</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <v>5.85</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="7">
         <v>8.0500000000000007</v>
       </c>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
-      <c r="A4" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="16" customHeight="1">
+      <c r="A4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <v>42703</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="22">
         <v>12</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="22">
         <v>23</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>19</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <f>D4+H4</f>
         <v>42722</v>
       </c>
-      <c r="J4" s="11">
-        <f t="shared" si="0"/>
+      <c r="J4" s="10">
+        <f>H4/4.5+30</f>
         <v>34.222222222222221</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="22">
         <v>0.129</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="22">
         <v>5.08</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="22">
         <v>9.0299999999999994</v>
       </c>
-      <c r="N4" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="4" customFormat="1" ht="16" customHeight="1">
-      <c r="A5" t="s">
+      <c r="N4" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" ht="16" customHeight="1">
+      <c r="A5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="20">
+        <v>42696</v>
+      </c>
+      <c r="E5" s="7">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7">
+        <v>23</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>31</v>
+      </c>
+      <c r="I5" s="8">
+        <v>42727</v>
+      </c>
+      <c r="J5" s="10">
+        <f>H5/4.5+30</f>
+        <v>36.888888888888886</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="L5" s="19">
+        <v>4.93</v>
+      </c>
+      <c r="M5" s="19">
+        <v>8.52</v>
+      </c>
+      <c r="N5" s="19"/>
+    </row>
+    <row r="6" spans="1:14" ht="16" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="8">
+        <v>42698</v>
+      </c>
+      <c r="E6" s="7">
+        <v>17</v>
+      </c>
+      <c r="F6" s="7">
+        <v>23</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>31</v>
+      </c>
+      <c r="I6" s="8">
+        <v>42729</v>
+      </c>
+      <c r="J6" s="10">
+        <f>H6/4.5+30</f>
+        <v>36.888888888888886</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="L6" s="7">
+        <v>5.52</v>
+      </c>
+      <c r="M6" s="7">
+        <v>8.64</v>
+      </c>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="8">
+        <v>42704</v>
+      </c>
+      <c r="E7" s="7">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>27</v>
+      </c>
+      <c r="I7" s="8">
+        <v>42731</v>
+      </c>
+      <c r="J7" s="10">
+        <f>H7/4.5+30</f>
+        <v>36</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="L7" s="7">
+        <v>5.79</v>
+      </c>
+      <c r="M7" s="7">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" customHeight="1">
+      <c r="A8" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="21">
+        <v>42698</v>
+      </c>
+      <c r="E8" s="16">
+        <v>17</v>
+      </c>
+      <c r="F8" s="16">
+        <v>23</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>36</v>
+      </c>
+      <c r="I8" s="8">
+        <v>42732</v>
+      </c>
+      <c r="J8" s="10">
+        <f>H8/4.5+30</f>
+        <v>38</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="L8" s="16">
+        <v>8.17</v>
+      </c>
+      <c r="M8" s="16">
+        <v>8.61</v>
+      </c>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" ht="16" customHeight="1">
+      <c r="A9" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="29">
+        <v>42701</v>
+      </c>
+      <c r="E9" s="22">
+        <v>14</v>
+      </c>
+      <c r="F9" s="22">
+        <v>23</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>32</v>
+      </c>
+      <c r="I9" s="9">
+        <f>D9+32</f>
+        <v>42733</v>
+      </c>
+      <c r="J9" s="10">
+        <f>H9/4.5+30</f>
+        <v>37.111111111111114</v>
+      </c>
+      <c r="K9" s="28">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="L9" s="28">
+        <v>5.66</v>
+      </c>
+      <c r="M9" s="28">
+        <v>8.14</v>
+      </c>
+      <c r="N9" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" customHeight="1">
+      <c r="A10" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="29">
+      <c r="C10" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="27">
+        <v>42698</v>
+      </c>
+      <c r="E10" s="26">
+        <v>17</v>
+      </c>
+      <c r="F10" s="26">
+        <v>23</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>34</v>
+      </c>
+      <c r="I10" s="8">
+        <v>42733</v>
+      </c>
+      <c r="J10" s="10">
+        <f>H10/4.5+30</f>
+        <v>37.555555555555557</v>
+      </c>
+      <c r="K10" s="26">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="L10" s="26">
+        <v>5.72</v>
+      </c>
+      <c r="M10" s="26">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" ht="16" customHeight="1">
+      <c r="A11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="21">
+        <v>42698</v>
+      </c>
+      <c r="E11" s="16">
+        <v>17</v>
+      </c>
+      <c r="F11" s="16">
+        <v>23</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>27</v>
+      </c>
+      <c r="I11" s="8">
+        <v>42740</v>
+      </c>
+      <c r="J11" s="10">
+        <f>H11/4.5+30</f>
+        <v>36</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.186</v>
+      </c>
+      <c r="L11" s="16">
+        <v>6.54</v>
+      </c>
+      <c r="M11" s="16">
+        <v>8.26</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" customFormat="1" ht="16" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="21">
         <v>42701</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E12" s="16">
         <v>14</v>
       </c>
-      <c r="F5" s="24">
-        <v>23</v>
-      </c>
-      <c r="G5" s="8">
+      <c r="F12" s="16">
+        <v>29</v>
+      </c>
+      <c r="G12" s="22">
         <v>1</v>
       </c>
-      <c r="H5" s="8">
-        <v>32</v>
-      </c>
-      <c r="I5" s="10">
-        <f>D5+32</f>
-        <v>42733</v>
-      </c>
-      <c r="J5" s="11">
-        <f t="shared" si="0"/>
-        <v>37.111111111111114</v>
-      </c>
-      <c r="K5">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="L5">
-        <v>5.66</v>
-      </c>
-      <c r="M5">
-        <v>8.14</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="16" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="H12" s="22">
         <v>15</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="9">
-        <v>42696</v>
-      </c>
-      <c r="E6" s="8">
-        <v>19</v>
-      </c>
-      <c r="F6" s="8">
-        <v>23</v>
-      </c>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
-        <v>31</v>
-      </c>
-      <c r="I6" s="9">
-        <v>42727</v>
-      </c>
-      <c r="J6" s="11">
-        <f t="shared" si="0"/>
-        <v>36.888888888888886</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="L6" s="8">
-        <v>4.93</v>
-      </c>
-      <c r="M6" s="8">
-        <v>8.52</v>
-      </c>
-      <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" ht="16" customHeight="1">
-      <c r="A7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="9">
-        <v>42698</v>
-      </c>
-      <c r="E7" s="8">
-        <v>17</v>
-      </c>
-      <c r="F7" s="8">
-        <v>23</v>
-      </c>
-      <c r="G7" s="8">
-        <v>2</v>
-      </c>
-      <c r="H7" s="8">
-        <v>31</v>
-      </c>
-      <c r="I7" s="9">
-        <v>42729</v>
-      </c>
-      <c r="J7" s="11">
-        <f t="shared" si="0"/>
-        <v>36.888888888888886</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="L7" s="8">
-        <v>5.52</v>
-      </c>
-      <c r="M7" s="8">
-        <v>8.64</v>
-      </c>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" ht="16" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9">
-        <v>42704</v>
-      </c>
-      <c r="E8" s="8">
-        <v>11</v>
-      </c>
-      <c r="F8" s="8">
-        <v>23</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2</v>
-      </c>
-      <c r="H8" s="8">
-        <v>27</v>
-      </c>
-      <c r="I8" s="9">
-        <v>42731</v>
-      </c>
-      <c r="J8" s="11">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="K8" s="8">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="L8" s="8">
-        <v>5.79</v>
-      </c>
-      <c r="M8" s="8">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="16" customHeight="1">
-      <c r="A9" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="23">
-        <v>42698</v>
-      </c>
-      <c r="E9" s="17">
-        <v>17</v>
-      </c>
-      <c r="F9" s="17">
-        <v>23</v>
-      </c>
-      <c r="G9" s="8">
-        <v>2</v>
-      </c>
-      <c r="H9" s="8">
-        <v>36</v>
-      </c>
-      <c r="I9" s="9">
-        <v>42732</v>
-      </c>
-      <c r="J9" s="11">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="K9" s="17">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="L9" s="17">
-        <v>8.17</v>
-      </c>
-      <c r="M9" s="17">
-        <v>8.61</v>
-      </c>
-      <c r="N9" s="12"/>
-    </row>
-    <row r="10" spans="1:14" ht="16" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="9">
-        <v>42705</v>
-      </c>
-      <c r="E10" s="8">
-        <v>10</v>
-      </c>
-      <c r="F10" s="8">
-        <v>23</v>
-      </c>
-      <c r="G10" s="8">
-        <v>2</v>
-      </c>
-      <c r="H10" s="8">
-        <v>34</v>
-      </c>
-      <c r="I10" s="9">
-        <v>42739</v>
-      </c>
-      <c r="J10" s="11">
-        <f t="shared" si="0"/>
-        <v>37.555555555555557</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0.122</v>
-      </c>
-      <c r="L10" s="8">
-        <v>5.27</v>
-      </c>
-      <c r="M10" s="8">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="16" customHeight="1">
-      <c r="A11" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="23">
-        <v>42698</v>
-      </c>
-      <c r="E11" s="17">
-        <v>17</v>
-      </c>
-      <c r="F11" s="17">
-        <v>23</v>
-      </c>
-      <c r="G11" s="8">
-        <v>2</v>
-      </c>
-      <c r="H11" s="8">
-        <v>27</v>
-      </c>
-      <c r="I11" s="9">
-        <v>42740</v>
-      </c>
-      <c r="J11" s="11">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="K11" s="17">
-        <v>0.186</v>
-      </c>
-      <c r="L11" s="17">
-        <v>6.54</v>
-      </c>
-      <c r="M11" s="17">
-        <v>8.26</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" customFormat="1" ht="16" customHeight="1">
-      <c r="A12" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="23">
-        <v>42701</v>
-      </c>
-      <c r="E12" s="17">
-        <v>14</v>
-      </c>
-      <c r="F12" s="17">
-        <v>29</v>
-      </c>
-      <c r="G12" s="24">
-        <v>1</v>
-      </c>
-      <c r="H12" s="24">
-        <v>15</v>
-      </c>
-      <c r="I12" s="25">
+      <c r="I12" s="23">
         <f>D12+H12</f>
         <v>42716</v>
       </c>
-      <c r="J12" s="26">
-        <f t="shared" ref="J12:J21" si="1">H12/2.6+30</f>
+      <c r="J12" s="24">
+        <f>H12/2.6+30</f>
         <v>35.769230769230766</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="16">
         <v>0.127</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12" s="16">
         <v>5.27</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="16">
         <v>8.19</v>
       </c>
-      <c r="N12" s="18" t="s">
-        <v>69</v>
+      <c r="N12" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:14" customFormat="1" ht="16" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="A13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="21">
         <v>42694</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>21</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="18">
         <v>29</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <v>2</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>22</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <f>D13+22</f>
         <v>42716</v>
       </c>
-      <c r="J13" s="11">
-        <f t="shared" si="1"/>
+      <c r="J13" s="10">
+        <f>H13/2.6+30</f>
         <v>38.46153846153846</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="16">
         <v>0.108</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="16">
         <v>5.47</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="16">
         <v>7.39</v>
       </c>
-      <c r="N13" s="24"/>
+      <c r="N13" s="22"/>
     </row>
     <row r="14" spans="1:14" ht="16" customHeight="1">
-      <c r="A14" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="23">
         <v>42698</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="22">
         <v>17</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="22">
         <v>29</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="22">
         <v>1</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="22">
         <v>19</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="23">
         <f>D14+H14</f>
         <v>42717</v>
       </c>
-      <c r="J14" s="26">
-        <f t="shared" si="1"/>
+      <c r="J14" s="24">
+        <f>H14/2.6+30</f>
         <v>37.307692307692307</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="22">
         <v>0.115</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="22">
         <v>5.23</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="22">
         <v>7.67</v>
       </c>
-      <c r="N14" s="24"/>
+      <c r="N14" s="22"/>
     </row>
     <row r="15" spans="1:14" ht="16" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="8">
+        <v>42702</v>
+      </c>
+      <c r="E15" s="7">
+        <v>13</v>
+      </c>
+      <c r="F15" s="7">
+        <v>29</v>
+      </c>
+      <c r="G15" s="7">
+        <v>2</v>
+      </c>
+      <c r="H15" s="7">
+        <v>18</v>
+      </c>
+      <c r="I15" s="8">
+        <v>42720</v>
+      </c>
+      <c r="J15" s="10">
+        <f>H15/2.6+30</f>
+        <v>36.92307692307692</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0.152</v>
+      </c>
+      <c r="L15" s="7">
+        <v>6.01</v>
+      </c>
+      <c r="M15" s="7">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="16" customHeight="1">
+      <c r="A16" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="29">
+        <v>42705</v>
+      </c>
+      <c r="E16" s="28">
+        <v>10</v>
+      </c>
+      <c r="F16" s="28">
+        <v>29</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="7">
+        <v>15</v>
+      </c>
+      <c r="I16" s="8">
+        <v>42720</v>
+      </c>
+      <c r="J16" s="10">
+        <f>H16/2.6+30</f>
+        <v>35.769230769230766</v>
+      </c>
+      <c r="K16" s="28">
+        <v>0.122</v>
+      </c>
+      <c r="L16" s="28">
+        <v>5.18</v>
+      </c>
+      <c r="M16" s="28">
+        <v>8.86</v>
+      </c>
+      <c r="N16" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="16" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="13">
+        <v>42709</v>
+      </c>
+      <c r="E17" s="14">
+        <v>6</v>
+      </c>
+      <c r="F17" s="14">
+        <v>29</v>
+      </c>
+      <c r="G17" s="14">
+        <v>1</v>
+      </c>
+      <c r="H17" s="14">
+        <v>12</v>
+      </c>
+      <c r="I17" s="15">
+        <f>D17+12</f>
+        <v>42721</v>
+      </c>
+      <c r="J17" s="10">
+        <f>H17/2.6+30</f>
+        <v>34.615384615384613</v>
+      </c>
+      <c r="K17" s="16">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L17" s="16">
+        <v>5.69</v>
+      </c>
+      <c r="M17" s="16">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="N17" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16" customHeight="1">
+      <c r="A18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="9">
-        <v>42702</v>
-      </c>
-      <c r="E15" s="8">
-        <v>13</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="D18" s="8">
+        <v>42706</v>
+      </c>
+      <c r="E18" s="7">
+        <v>9</v>
+      </c>
+      <c r="F18" s="7">
         <v>29</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G18" s="7">
         <v>2</v>
       </c>
-      <c r="H15" s="8">
-        <v>18</v>
-      </c>
-      <c r="I15" s="9">
-        <v>42720</v>
-      </c>
-      <c r="J15" s="11">
-        <f t="shared" si="1"/>
-        <v>36.92307692307692</v>
-      </c>
-      <c r="K15" s="8">
-        <v>0.152</v>
-      </c>
-      <c r="L15" s="8">
-        <v>6.01</v>
-      </c>
-      <c r="M15" s="8">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="16" customHeight="1">
-      <c r="A16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="14">
-        <v>42709</v>
-      </c>
-      <c r="E16" s="15">
-        <v>6</v>
-      </c>
-      <c r="F16" s="15">
+      <c r="H18" s="7">
+        <v>17</v>
+      </c>
+      <c r="I18" s="8">
+        <v>42723</v>
+      </c>
+      <c r="J18" s="10">
+        <f>H18/2.6+30</f>
+        <v>36.53846153846154</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0.155</v>
+      </c>
+      <c r="L18" s="7">
+        <v>5.93</v>
+      </c>
+      <c r="M18" s="7">
+        <v>7.98</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="16" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="8">
+        <v>42708</v>
+      </c>
+      <c r="E19" s="7">
+        <v>7</v>
+      </c>
+      <c r="F19" s="7">
         <v>29</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G19" s="7">
+        <v>2</v>
+      </c>
+      <c r="H19" s="7">
+        <v>17</v>
+      </c>
+      <c r="I19" s="8">
+        <v>42725</v>
+      </c>
+      <c r="J19" s="10">
+        <f>H19/2.6+30</f>
+        <v>36.53846153846154</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0.121</v>
+      </c>
+      <c r="L19" s="7">
+        <v>5.58</v>
+      </c>
+      <c r="M19" s="7">
+        <v>7.33</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16" customHeight="1">
+      <c r="A20" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="32">
+        <v>42714</v>
+      </c>
+      <c r="E20" s="33">
         <v>1</v>
       </c>
-      <c r="H16" s="15">
+      <c r="F20" s="34">
+        <v>29</v>
+      </c>
+      <c r="G20" s="33">
+        <v>1</v>
+      </c>
+      <c r="H20" s="33">
         <v>12</v>
       </c>
-      <c r="I16" s="16">
-        <f>D16+12</f>
-        <v>42721</v>
-      </c>
-      <c r="J16" s="11">
-        <f t="shared" si="1"/>
-        <v>34.615384615384613</v>
-      </c>
-      <c r="K16" s="17">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="L16" s="17">
-        <v>5.69</v>
-      </c>
-      <c r="M16" s="17">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="N16" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="16" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="9">
-        <v>42706</v>
-      </c>
-      <c r="E17" s="8">
-        <v>9</v>
-      </c>
-      <c r="F17" s="8">
-        <v>29</v>
-      </c>
-      <c r="G17" s="8">
-        <v>2</v>
-      </c>
-      <c r="H17" s="8">
-        <v>17</v>
-      </c>
-      <c r="I17" s="9">
-        <v>42723</v>
-      </c>
-      <c r="J17" s="11">
-        <f t="shared" si="1"/>
-        <v>36.53846153846154</v>
-      </c>
-      <c r="K17" s="8">
-        <v>0.155</v>
-      </c>
-      <c r="L17" s="8">
-        <v>5.93</v>
-      </c>
-      <c r="M17" s="8">
-        <v>7.98</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="16" customHeight="1">
-      <c r="A18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="14">
-        <v>42710</v>
-      </c>
-      <c r="E18" s="15">
-        <v>5</v>
-      </c>
-      <c r="F18" s="19">
-        <v>29</v>
-      </c>
-      <c r="G18" s="15">
-        <v>1</v>
-      </c>
-      <c r="H18" s="15">
-        <v>14</v>
-      </c>
-      <c r="I18" s="16">
-        <f>D18+14</f>
-        <v>42724</v>
-      </c>
-      <c r="J18" s="11">
-        <f t="shared" si="1"/>
-        <v>35.384615384615387</v>
-      </c>
-      <c r="K18" s="17">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="L18" s="17">
-        <v>5.83</v>
-      </c>
-      <c r="M18" s="17">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="16" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="9">
-        <v>42708</v>
-      </c>
-      <c r="E19" s="8">
-        <v>7</v>
-      </c>
-      <c r="F19" s="8">
-        <v>29</v>
-      </c>
-      <c r="G19" s="8">
-        <v>2</v>
-      </c>
-      <c r="H19" s="8">
-        <v>17</v>
-      </c>
-      <c r="I19" s="9">
-        <v>42725</v>
-      </c>
-      <c r="J19" s="11">
-        <f t="shared" si="1"/>
-        <v>36.53846153846154</v>
-      </c>
-      <c r="K19" s="8">
-        <v>0.121</v>
-      </c>
-      <c r="L19" s="8">
-        <v>5.58</v>
-      </c>
-      <c r="M19" s="8">
-        <v>7.33</v>
-      </c>
-      <c r="N19" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="16" customHeight="1">
-      <c r="A20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="14">
-        <v>42714</v>
-      </c>
-      <c r="E20" s="15">
-        <v>1</v>
-      </c>
-      <c r="F20" s="19">
-        <v>29</v>
-      </c>
-      <c r="G20" s="15">
-        <v>1</v>
-      </c>
-      <c r="H20" s="15">
-        <v>12</v>
-      </c>
-      <c r="I20" s="16">
+      <c r="I20" s="35">
         <f>D20+12</f>
         <v>42726</v>
       </c>
-      <c r="J20" s="11">
-        <f t="shared" si="1"/>
+      <c r="J20" s="36">
+        <f>H20/2.6+30</f>
         <v>34.615384615384613</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="37">
         <v>0.13400000000000001</v>
       </c>
-      <c r="L20" s="17">
+      <c r="L20" s="37">
         <v>5.36</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="37">
         <v>8.35</v>
       </c>
-      <c r="N20" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="16" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="N20" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="39" customFormat="1" ht="16" customHeight="1">
+      <c r="A21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="8">
+        <v>42711</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4</v>
+      </c>
+      <c r="F21" s="7">
+        <v>29</v>
+      </c>
+      <c r="G21" s="7">
+        <v>2</v>
+      </c>
+      <c r="H21" s="7">
+        <v>18</v>
+      </c>
+      <c r="I21" s="8">
+        <v>42729</v>
+      </c>
+      <c r="J21" s="10">
+        <f>H21/2.6+30</f>
+        <v>36.92307692307692</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0.129</v>
+      </c>
+      <c r="L21" s="7">
+        <v>5.44</v>
+      </c>
+      <c r="M21" s="7">
+        <v>8.76</v>
+      </c>
+      <c r="N21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="9">
-        <v>42711</v>
-      </c>
-      <c r="E21" s="8">
-        <v>4</v>
-      </c>
-      <c r="F21" s="8">
-        <v>29</v>
-      </c>
-      <c r="G21" s="8">
-        <v>2</v>
-      </c>
-      <c r="H21" s="8">
-        <v>18</v>
-      </c>
-      <c r="I21" s="9">
-        <v>42729</v>
-      </c>
-      <c r="J21" s="11">
-        <f t="shared" si="1"/>
-        <v>36.92307692307692</v>
-      </c>
-      <c r="K21" s="8">
-        <v>0.129</v>
-      </c>
-      <c r="L21" s="8">
-        <v>5.44</v>
-      </c>
-      <c r="M21" s="8">
-        <v>8.76</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="22" spans="1:14" ht="16" customHeight="1">
-      <c r="A22" s="31"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2">
-        <f>AVERAGE(H3:H21)</f>
-        <v>22.631578947368421</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2">
-        <f>AVERAGE(J3:J21)</f>
-        <v>36.430949167791276</v>
-      </c>
-      <c r="K22" s="20">
-        <f>AVERAGE(K3:K21)</f>
-        <v>0.13705263157894734</v>
-      </c>
-      <c r="L22" s="1">
-        <f>AVERAGE(L3:L21)</f>
-        <v>5.7168421052631571</v>
-      </c>
-      <c r="M22" s="1">
-        <f>AVERAGE(M3:M21)</f>
-        <v>8.3052631578947373</v>
-      </c>
-      <c r="N22" s="27"/>
-    </row>
-    <row r="23" spans="1:14" ht="16" customHeight="1">
-      <c r="A23" s="32"/>
+      <c r="A22" s="19"/>
+    </row>
+    <row r="23" spans="1:14" customFormat="1" ht="16" customHeight="1">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:N22">
-    <sortCondition ref="F2:F22"/>
-    <sortCondition ref="I2:I22"/>
+  <sortState ref="A2:N25">
+    <sortCondition ref="F2:F25"/>
+    <sortCondition ref="I2:I25"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B22:B1048576 B1 B4 B12 B10 B14:B20 B6:B8">
+  <conditionalFormatting sqref="B24:B1048576 B21:B22 B1 B4 B12 B14:B19 B6:B8">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
+  <conditionalFormatting sqref="B20">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
@@ -2052,7 +2064,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="84" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="99" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>